<commit_message>
commit on 16th Final
</commit_message>
<xml_diff>
--- a/Seq_Hyd_Maven_Proj/TestData/Test_Scenario.xlsx
+++ b/Seq_Hyd_Maven_Proj/TestData/Test_Scenario.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Keyword_Scenario" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Application_Submit</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>TestCase_3</t>
+  </si>
+  <si>
+    <t>Application_Submit1</t>
   </si>
 </sst>
 </file>
@@ -400,8 +403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +446,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
@@ -454,7 +457,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -469,7 +472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>